<commit_message>
end of night, added accelerometer to main_controller & verified working circuit boards
</commit_message>
<xml_diff>
--- a/lab/7/arduino_code/extras/Segment and Accelerometer Pinout.xlsx
+++ b/lab/7/arduino_code/extras/Segment and Accelerometer Pinout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA6B34-E551-409B-8BEB-ACAD62E103B4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6ED069BB-2ED1-4AC5-AD1E-CF1BD984A4ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,8 +141,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3554186</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>31406</xdr:rowOff>
     </xdr:to>
@@ -452,17 +452,19 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.61328125" customWidth="1"/>
-    <col min="3" max="3" width="51.69140625" customWidth="1"/>
-    <col min="4" max="4" width="18.53515625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -476,7 +478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -490,7 +492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -504,7 +506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -518,7 +520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -532,7 +534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -540,7 +542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -548,7 +550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -556,7 +558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -564,7 +566,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -572,7 +574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -580,7 +582,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>

</xml_diff>